<commit_message>
Completando tarea parte 0
</commit_message>
<xml_diff>
--- a/Html.xlsx
+++ b/Html.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e9259bd8aba9c992/Documentos/Cursos/FullstackOpen/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="190" documentId="11_AD4D2F04E46CFB4ACB3E20A05517F712683EDF1D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B78696A6-EC40-42BE-9EF9-B641185A5ACF}"/>
+  <xr:revisionPtr revIDLastSave="191" documentId="11_AD4D2F04E46CFB4ACB3E20A05517F712683EDF1D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{32C5C937-C7B3-4520-B7BA-1C44DE61C1C5}"/>
   <bookViews>
-    <workbookView xWindow="29760" yWindow="960" windowWidth="21600" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="152">
   <si>
     <t>Etiquetas Html</t>
   </si>
@@ -555,6 +555,9 @@
   </si>
   <si>
     <t>…or push an existing repository from the command line</t>
+  </si>
+  <si>
+    <t>git status</t>
   </si>
 </sst>
 </file>
@@ -690,6 +693,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="distributed"/>
     </xf>
@@ -707,13 +717,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="distributed"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -756,7 +759,7 @@
         <xdr:cNvPr id="2" name="Imagen 1" descr="elementos de gato gruñon">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C3225AF3-0C64-2014-3E6F-5026695F6072}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -817,7 +820,7 @@
         <xdr:cNvPr id="3" name="Imagen 2" descr="atributo html">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{77CA768E-046C-C190-31EB-AF6BC4445E7C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -878,7 +881,7 @@
         <xdr:cNvPr id="4" name="Imagen 3" descr="Partes de una declaracion de css">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C2060973-A2C2-1F95-3C59-47B1BDF46C37}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -939,7 +942,7 @@
         <xdr:cNvPr id="5" name="Imagen 4" descr="tres cajas puestas una dentro de otra. De fuera a dentro están etiquetadas con el margen, el borde y el relleno">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BB49706D-4166-252F-8386-A541333AF489}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1005,7 +1008,7 @@
                   <a14:compatExt spid="_x0000_s1025"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D972F85E-411B-0647-D649-04D13FC4B981}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1305,8 +1308,8 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:L190"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A160" workbookViewId="0">
-      <selection activeCell="E172" sqref="E172"/>
+    <sheetView tabSelected="1" topLeftCell="A174" workbookViewId="0">
+      <selection activeCell="F180" sqref="F180"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -1826,10 +1829,10 @@
       </c>
     </row>
     <row r="128" spans="1:12">
-      <c r="J128" s="9" t="s">
+      <c r="J128" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="K128" s="7" t="s">
+      <c r="K128" s="10" t="s">
         <v>104</v>
       </c>
       <c r="L128" s="5" t="s">
@@ -1837,17 +1840,17 @@
       </c>
     </row>
     <row r="129" spans="1:12">
-      <c r="J129" s="10"/>
-      <c r="K129" s="8"/>
+      <c r="J129" s="13"/>
+      <c r="K129" s="11"/>
       <c r="L129" s="4" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="130" spans="1:12">
-      <c r="J130" s="7" t="s">
+      <c r="J130" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="K130" s="9" t="s">
+      <c r="K130" s="12" t="s">
         <v>107</v>
       </c>
       <c r="L130" s="5" t="s">
@@ -1855,17 +1858,17 @@
       </c>
     </row>
     <row r="131" spans="1:12">
-      <c r="J131" s="8"/>
-      <c r="K131" s="10"/>
+      <c r="J131" s="11"/>
+      <c r="K131" s="13"/>
       <c r="L131" s="4" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="132" spans="1:12">
-      <c r="J132" s="7" t="s">
+      <c r="J132" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="K132" s="7" t="s">
+      <c r="K132" s="10" t="s">
         <v>110</v>
       </c>
       <c r="L132" s="5" t="s">
@@ -1873,17 +1876,17 @@
       </c>
     </row>
     <row r="133" spans="1:12">
-      <c r="J133" s="8"/>
-      <c r="K133" s="8"/>
+      <c r="J133" s="11"/>
+      <c r="K133" s="11"/>
       <c r="L133" s="2" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="134" spans="1:12">
-      <c r="J134" s="7" t="s">
+      <c r="J134" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="K134" s="7" t="s">
+      <c r="K134" s="10" t="s">
         <v>113</v>
       </c>
       <c r="L134" s="5" t="s">
@@ -1891,17 +1894,17 @@
       </c>
     </row>
     <row r="135" spans="1:12">
-      <c r="J135" s="8"/>
-      <c r="K135" s="8"/>
+      <c r="J135" s="11"/>
+      <c r="K135" s="11"/>
       <c r="L135" s="2" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="136" spans="1:12">
-      <c r="J136" s="7" t="s">
+      <c r="J136" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="K136" s="11" t="s">
+      <c r="K136" s="14" t="s">
         <v>116</v>
       </c>
       <c r="L136" s="5" t="s">
@@ -1909,8 +1912,8 @@
       </c>
     </row>
     <row r="137" spans="1:12">
-      <c r="J137" s="8"/>
-      <c r="K137" s="12"/>
+      <c r="J137" s="11"/>
+      <c r="K137" s="15"/>
       <c r="L137" s="6" t="s">
         <v>122</v>
       </c>
@@ -2002,12 +2005,12 @@
       </c>
     </row>
     <row r="169" spans="1:1" ht="18">
-      <c r="A169" s="13" t="s">
+      <c r="A169" s="7" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="171" spans="1:1">
-      <c r="A171" s="14" t="s">
+      <c r="A171" s="8" t="s">
         <v>140</v>
       </c>
     </row>
@@ -2017,62 +2020,65 @@
       </c>
     </row>
     <row r="176" spans="1:1" ht="18">
-      <c r="A176" s="13" t="s">
+      <c r="A176" s="7" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="178" spans="1:1" ht="15">
-      <c r="A178" s="15" t="s">
+    <row r="178" spans="1:6" ht="15">
+      <c r="A178" s="9" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="179" spans="1:1" ht="15">
-      <c r="A179" s="15" t="s">
+    <row r="179" spans="1:6" ht="15">
+      <c r="A179" s="9" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="180" spans="1:1" ht="15">
-      <c r="A180" s="15" t="s">
+      <c r="F179" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="180" spans="1:6" ht="15">
+      <c r="A180" s="9" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="181" spans="1:1" ht="15">
-      <c r="A181" s="15" t="s">
+    <row r="181" spans="1:6" ht="15">
+      <c r="A181" s="9" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="182" spans="1:1" ht="15">
-      <c r="A182" s="15" t="s">
+    <row r="182" spans="1:6" ht="15">
+      <c r="A182" s="9" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="183" spans="1:1" ht="15">
-      <c r="A183" s="15" t="s">
+    <row r="183" spans="1:6" ht="15">
+      <c r="A183" s="9" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="184" spans="1:1" ht="15">
-      <c r="A184" s="15" t="s">
+    <row r="184" spans="1:6" ht="15">
+      <c r="A184" s="9" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="186" spans="1:1" ht="18">
-      <c r="A186" s="13" t="s">
+    <row r="186" spans="1:6" ht="18">
+      <c r="A186" s="7" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="188" spans="1:1" ht="15">
-      <c r="A188" s="15" t="s">
+    <row r="188" spans="1:6" ht="15">
+      <c r="A188" s="9" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="189" spans="1:1" ht="15">
-      <c r="A189" s="15" t="s">
+    <row r="189" spans="1:6" ht="15">
+      <c r="A189" s="9" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="190" spans="1:1" ht="15">
-      <c r="A190" s="15" t="s">
+    <row r="190" spans="1:6" ht="15">
+      <c r="A190" s="9" t="s">
         <v>149</v>
       </c>
     </row>

</xml_diff>